<commit_message>
updated for c not in feeder fuck u
</commit_message>
<xml_diff>
--- a/Output/Scenario_0.35_3500_0_0_0_0_0_0_.xlsx
+++ b/Output/Scenario_0.35_3500_0_0_0_0_0_0_.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d97d3de92643fad0/Documents/Documents/Mestrado/PlanejamentoEstocasticoDeRotas/Output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="11_258DEA403018A65302F20A5EA041B45A3CCF5C43" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{80A10AD8-5F1B-4AD5-A112-BCB5D129DC00}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="11_258DEA403018A65302F20A5EA041B45A3CCF5C43" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BBBC3D45-0332-4E79-B9E4-23EFE5C5937F}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -278,12 +278,18 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -313,13 +319,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -11635,6 +11644,112 @@
     </row>
   </sheetData>
   <mergeCells count="130">
+    <mergeCell ref="C200:C201"/>
+    <mergeCell ref="A162:A201"/>
+    <mergeCell ref="C92:C93"/>
+    <mergeCell ref="C196:C197"/>
+    <mergeCell ref="C88:C89"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="B66:B73"/>
+    <mergeCell ref="C124:C125"/>
+    <mergeCell ref="C180:C181"/>
+    <mergeCell ref="C118:C119"/>
+    <mergeCell ref="C198:C199"/>
+    <mergeCell ref="A42:A81"/>
+    <mergeCell ref="C90:C91"/>
+    <mergeCell ref="B130:B137"/>
+    <mergeCell ref="C130:C131"/>
+    <mergeCell ref="C182:C183"/>
+    <mergeCell ref="C52:C53"/>
+    <mergeCell ref="C110:C111"/>
+    <mergeCell ref="C150:C151"/>
+    <mergeCell ref="C72:C73"/>
+    <mergeCell ref="C96:C97"/>
+    <mergeCell ref="C158:C159"/>
+    <mergeCell ref="C136:C137"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="C194:C195"/>
+    <mergeCell ref="C122:C123"/>
+    <mergeCell ref="C178:C179"/>
+    <mergeCell ref="A82:A121"/>
+    <mergeCell ref="C78:C79"/>
+    <mergeCell ref="B178:B185"/>
+    <mergeCell ref="C172:C173"/>
+    <mergeCell ref="A122:A161"/>
+    <mergeCell ref="B186:B193"/>
+    <mergeCell ref="B162:B169"/>
+    <mergeCell ref="C170:C171"/>
+    <mergeCell ref="C64:C65"/>
+    <mergeCell ref="B74:B81"/>
+    <mergeCell ref="C154:C155"/>
+    <mergeCell ref="B114:B121"/>
+    <mergeCell ref="B154:B161"/>
+    <mergeCell ref="C104:C105"/>
+    <mergeCell ref="B138:B145"/>
+    <mergeCell ref="C156:C157"/>
+    <mergeCell ref="C142:C143"/>
+    <mergeCell ref="C80:C81"/>
+    <mergeCell ref="B170:B177"/>
+    <mergeCell ref="C108:C109"/>
+    <mergeCell ref="C160:C161"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="C192:C193"/>
+    <mergeCell ref="C144:C145"/>
+    <mergeCell ref="C36:C37"/>
+    <mergeCell ref="C176:C177"/>
+    <mergeCell ref="C70:C71"/>
+    <mergeCell ref="C38:C39"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="C120:C121"/>
+    <mergeCell ref="C174:C175"/>
+    <mergeCell ref="C168:C169"/>
+    <mergeCell ref="C184:C185"/>
+    <mergeCell ref="C48:C49"/>
+    <mergeCell ref="C62:C63"/>
+    <mergeCell ref="C106:C107"/>
+    <mergeCell ref="C186:C187"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="C60:C61"/>
+    <mergeCell ref="B82:B89"/>
+    <mergeCell ref="C82:C83"/>
+    <mergeCell ref="C140:C141"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="B10:B17"/>
+    <mergeCell ref="B146:B153"/>
+    <mergeCell ref="C102:C103"/>
+    <mergeCell ref="B34:B41"/>
+    <mergeCell ref="C34:C35"/>
+    <mergeCell ref="C74:C75"/>
+    <mergeCell ref="C68:C69"/>
+    <mergeCell ref="C126:C127"/>
+    <mergeCell ref="C58:C59"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="C116:C117"/>
+    <mergeCell ref="C42:C43"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="C50:C51"/>
+    <mergeCell ref="C44:C45"/>
+    <mergeCell ref="C84:C85"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="C94:C95"/>
+    <mergeCell ref="C40:C41"/>
+    <mergeCell ref="B58:B65"/>
+    <mergeCell ref="C138:C139"/>
+    <mergeCell ref="B98:B105"/>
+    <mergeCell ref="C76:C77"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="C128:C129"/>
+    <mergeCell ref="B26:B33"/>
+    <mergeCell ref="C146:C147"/>
+    <mergeCell ref="B122:B129"/>
+    <mergeCell ref="C54:C55"/>
+    <mergeCell ref="C112:C113"/>
+    <mergeCell ref="B106:B113"/>
+    <mergeCell ref="C100:C101"/>
+    <mergeCell ref="C152:C153"/>
+    <mergeCell ref="C56:C57"/>
+    <mergeCell ref="C148:C149"/>
+    <mergeCell ref="C46:C47"/>
     <mergeCell ref="A2:A41"/>
     <mergeCell ref="B194:B201"/>
     <mergeCell ref="C10:C11"/>
@@ -11659,112 +11774,6 @@
     <mergeCell ref="C166:C167"/>
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="C162:C163"/>
-    <mergeCell ref="B122:B129"/>
-    <mergeCell ref="C54:C55"/>
-    <mergeCell ref="C112:C113"/>
-    <mergeCell ref="B106:B113"/>
-    <mergeCell ref="C100:C101"/>
-    <mergeCell ref="C152:C153"/>
-    <mergeCell ref="C56:C57"/>
-    <mergeCell ref="C148:C149"/>
-    <mergeCell ref="C46:C47"/>
-    <mergeCell ref="C40:C41"/>
-    <mergeCell ref="B58:B65"/>
-    <mergeCell ref="C138:C139"/>
-    <mergeCell ref="B98:B105"/>
-    <mergeCell ref="C76:C77"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="C128:C129"/>
-    <mergeCell ref="B26:B33"/>
-    <mergeCell ref="C146:C147"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="C60:C61"/>
-    <mergeCell ref="B82:B89"/>
-    <mergeCell ref="C82:C83"/>
-    <mergeCell ref="C140:C141"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="B10:B17"/>
-    <mergeCell ref="B146:B153"/>
-    <mergeCell ref="C102:C103"/>
-    <mergeCell ref="B34:B41"/>
-    <mergeCell ref="C34:C35"/>
-    <mergeCell ref="C74:C75"/>
-    <mergeCell ref="C68:C69"/>
-    <mergeCell ref="C126:C127"/>
-    <mergeCell ref="C58:C59"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="C116:C117"/>
-    <mergeCell ref="C42:C43"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="C50:C51"/>
-    <mergeCell ref="C44:C45"/>
-    <mergeCell ref="C84:C85"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="C94:C95"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="C192:C193"/>
-    <mergeCell ref="C144:C145"/>
-    <mergeCell ref="C36:C37"/>
-    <mergeCell ref="C176:C177"/>
-    <mergeCell ref="C70:C71"/>
-    <mergeCell ref="C38:C39"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="C120:C121"/>
-    <mergeCell ref="C174:C175"/>
-    <mergeCell ref="C168:C169"/>
-    <mergeCell ref="C184:C185"/>
-    <mergeCell ref="C48:C49"/>
-    <mergeCell ref="C62:C63"/>
-    <mergeCell ref="C106:C107"/>
-    <mergeCell ref="B162:B169"/>
-    <mergeCell ref="C170:C171"/>
-    <mergeCell ref="C64:C65"/>
-    <mergeCell ref="B74:B81"/>
-    <mergeCell ref="C154:C155"/>
-    <mergeCell ref="B114:B121"/>
-    <mergeCell ref="B154:B161"/>
-    <mergeCell ref="C104:C105"/>
-    <mergeCell ref="B138:B145"/>
-    <mergeCell ref="C156:C157"/>
-    <mergeCell ref="C142:C143"/>
-    <mergeCell ref="C80:C81"/>
-    <mergeCell ref="B170:B177"/>
-    <mergeCell ref="C108:C109"/>
-    <mergeCell ref="C186:C187"/>
-    <mergeCell ref="C160:C161"/>
-    <mergeCell ref="C194:C195"/>
-    <mergeCell ref="C122:C123"/>
-    <mergeCell ref="C178:C179"/>
-    <mergeCell ref="A82:A121"/>
-    <mergeCell ref="C78:C79"/>
-    <mergeCell ref="B178:B185"/>
-    <mergeCell ref="C172:C173"/>
-    <mergeCell ref="A122:A161"/>
-    <mergeCell ref="B186:B193"/>
-    <mergeCell ref="C200:C201"/>
-    <mergeCell ref="A162:A201"/>
-    <mergeCell ref="C92:C93"/>
-    <mergeCell ref="C196:C197"/>
-    <mergeCell ref="C88:C89"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="B66:B73"/>
-    <mergeCell ref="C124:C125"/>
-    <mergeCell ref="C180:C181"/>
-    <mergeCell ref="C118:C119"/>
-    <mergeCell ref="C198:C199"/>
-    <mergeCell ref="A42:A81"/>
-    <mergeCell ref="C90:C91"/>
-    <mergeCell ref="B130:B137"/>
-    <mergeCell ref="C130:C131"/>
-    <mergeCell ref="C182:C183"/>
-    <mergeCell ref="C52:C53"/>
-    <mergeCell ref="C110:C111"/>
-    <mergeCell ref="C150:C151"/>
-    <mergeCell ref="C72:C73"/>
-    <mergeCell ref="C96:C97"/>
-    <mergeCell ref="C158:C159"/>
-    <mergeCell ref="C136:C137"/>
-    <mergeCell ref="C28:C29"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -16187,20 +16196,6 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="B66:B69"/>
-    <mergeCell ref="B94:B97"/>
-    <mergeCell ref="B18:B21"/>
-    <mergeCell ref="B50:B53"/>
-    <mergeCell ref="B86:B89"/>
-    <mergeCell ref="B46:B49"/>
-    <mergeCell ref="B70:B73"/>
-    <mergeCell ref="B90:B93"/>
-    <mergeCell ref="B2:B5"/>
-    <mergeCell ref="A42:A61"/>
-    <mergeCell ref="B42:B45"/>
-    <mergeCell ref="B62:B65"/>
-    <mergeCell ref="B14:B17"/>
-    <mergeCell ref="B22:B25"/>
     <mergeCell ref="B98:B101"/>
     <mergeCell ref="A2:A21"/>
     <mergeCell ref="A62:A81"/>
@@ -16217,6 +16212,20 @@
     <mergeCell ref="B26:B29"/>
     <mergeCell ref="A82:A101"/>
     <mergeCell ref="B54:B57"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="A42:A61"/>
+    <mergeCell ref="B42:B45"/>
+    <mergeCell ref="B62:B65"/>
+    <mergeCell ref="B14:B17"/>
+    <mergeCell ref="B22:B25"/>
+    <mergeCell ref="B66:B69"/>
+    <mergeCell ref="B94:B97"/>
+    <mergeCell ref="B18:B21"/>
+    <mergeCell ref="B50:B53"/>
+    <mergeCell ref="B86:B89"/>
+    <mergeCell ref="B46:B49"/>
+    <mergeCell ref="B70:B73"/>
+    <mergeCell ref="B90:B93"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -17150,24 +17159,27 @@
   <dimension ref="A1:M18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15:L15"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="3" width="15.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.21875" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.21875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15.21875" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="16.21875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>25</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -17182,7 +17194,7 @@
       <c r="F1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="4" t="s">
         <v>45</v>
       </c>
       <c r="H1" s="1" t="s">
@@ -17194,7 +17206,7 @@
       <c r="J1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="4" t="s">
         <v>47</v>
       </c>
       <c r="L1" s="1" t="s">
@@ -54053,29 +54065,468 @@
     </row>
   </sheetData>
   <mergeCells count="510">
-    <mergeCell ref="C800:C801"/>
-    <mergeCell ref="C210:C211"/>
-    <mergeCell ref="C324:C325"/>
-    <mergeCell ref="B194:B201"/>
-    <mergeCell ref="C274:C275"/>
-    <mergeCell ref="B50:B57"/>
-    <mergeCell ref="C114:C115"/>
-    <mergeCell ref="B690:B697"/>
-    <mergeCell ref="C132:C133"/>
-    <mergeCell ref="C272:C273"/>
-    <mergeCell ref="C332:C333"/>
-    <mergeCell ref="C630:C631"/>
-    <mergeCell ref="C778:C779"/>
-    <mergeCell ref="C796:C797"/>
-    <mergeCell ref="C682:C683"/>
-    <mergeCell ref="C738:C739"/>
-    <mergeCell ref="B666:B673"/>
-    <mergeCell ref="C746:C747"/>
-    <mergeCell ref="B730:B737"/>
-    <mergeCell ref="B674:B681"/>
-    <mergeCell ref="C370:C371"/>
-    <mergeCell ref="C96:C97"/>
-    <mergeCell ref="C532:C533"/>
+    <mergeCell ref="C798:C799"/>
+    <mergeCell ref="C108:C109"/>
+    <mergeCell ref="B226:B233"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="C266:C267"/>
+    <mergeCell ref="C322:C323"/>
+    <mergeCell ref="C260:C261"/>
+    <mergeCell ref="C558:C559"/>
+    <mergeCell ref="A162:A241"/>
+    <mergeCell ref="B426:B433"/>
+    <mergeCell ref="C298:C299"/>
+    <mergeCell ref="C456:C457"/>
+    <mergeCell ref="C754:C755"/>
+    <mergeCell ref="C64:C65"/>
+    <mergeCell ref="C406:C407"/>
+    <mergeCell ref="C614:C615"/>
+    <mergeCell ref="B482:B489"/>
+    <mergeCell ref="C706:C707"/>
+    <mergeCell ref="C374:C375"/>
+    <mergeCell ref="C716:C717"/>
+    <mergeCell ref="C672:C673"/>
+    <mergeCell ref="C88:C89"/>
+    <mergeCell ref="C472:C473"/>
+    <mergeCell ref="C708:C709"/>
+    <mergeCell ref="A82:A161"/>
+    <mergeCell ref="A562:A641"/>
+    <mergeCell ref="A482:A561"/>
+    <mergeCell ref="C644:C645"/>
+    <mergeCell ref="A242:A321"/>
+    <mergeCell ref="C92:C93"/>
+    <mergeCell ref="B82:B89"/>
+    <mergeCell ref="C634:C635"/>
+    <mergeCell ref="B210:B217"/>
+    <mergeCell ref="B514:B521"/>
+    <mergeCell ref="B298:B305"/>
+    <mergeCell ref="A322:A401"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="C244:C245"/>
+    <mergeCell ref="C542:C543"/>
+    <mergeCell ref="C700:C701"/>
+    <mergeCell ref="C308:C309"/>
+    <mergeCell ref="C606:C607"/>
+    <mergeCell ref="C102:C103"/>
+    <mergeCell ref="C544:C545"/>
+    <mergeCell ref="B34:B41"/>
+    <mergeCell ref="C564:C565"/>
+    <mergeCell ref="C74:C75"/>
+    <mergeCell ref="C68:C69"/>
+    <mergeCell ref="C372:C373"/>
+    <mergeCell ref="C310:C311"/>
+    <mergeCell ref="B506:B513"/>
+    <mergeCell ref="C608:C609"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="C116:C117"/>
+    <mergeCell ref="B570:B577"/>
+    <mergeCell ref="B458:B465"/>
+    <mergeCell ref="B634:B641"/>
+    <mergeCell ref="B202:B209"/>
+    <mergeCell ref="C202:C203"/>
+    <mergeCell ref="C444:C445"/>
+    <mergeCell ref="B786:B793"/>
+    <mergeCell ref="C218:C219"/>
+    <mergeCell ref="C638:C639"/>
+    <mergeCell ref="C230:C231"/>
+    <mergeCell ref="C168:C169"/>
+    <mergeCell ref="C290:C291"/>
+    <mergeCell ref="C466:C467"/>
+    <mergeCell ref="C764:C765"/>
+    <mergeCell ref="C382:C383"/>
+    <mergeCell ref="C624:C625"/>
+    <mergeCell ref="B170:B177"/>
+    <mergeCell ref="C688:C689"/>
+    <mergeCell ref="C684:C685"/>
+    <mergeCell ref="C192:C193"/>
+    <mergeCell ref="C428:C429"/>
+    <mergeCell ref="C238:C239"/>
+    <mergeCell ref="C474:C475"/>
+    <mergeCell ref="C194:C195"/>
+    <mergeCell ref="C492:C493"/>
+    <mergeCell ref="C240:C241"/>
+    <mergeCell ref="C296:C297"/>
+    <mergeCell ref="C598:C599"/>
+    <mergeCell ref="B178:B185"/>
+    <mergeCell ref="C258:C259"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="C300:C301"/>
+    <mergeCell ref="C66:C67"/>
+    <mergeCell ref="C498:C499"/>
+    <mergeCell ref="C740:C741"/>
+    <mergeCell ref="B762:B769"/>
+    <mergeCell ref="B234:B241"/>
+    <mergeCell ref="B618:B625"/>
+    <mergeCell ref="C264:C265"/>
+    <mergeCell ref="B186:B193"/>
+    <mergeCell ref="C358:C359"/>
+    <mergeCell ref="C656:C657"/>
+    <mergeCell ref="C618:C619"/>
+    <mergeCell ref="C658:C659"/>
+    <mergeCell ref="C756:C757"/>
+    <mergeCell ref="C378:C379"/>
+    <mergeCell ref="C166:C167"/>
+    <mergeCell ref="C464:C465"/>
+    <mergeCell ref="C402:C403"/>
+    <mergeCell ref="C524:C525"/>
+    <mergeCell ref="C712:C713"/>
+    <mergeCell ref="B106:B113"/>
+    <mergeCell ref="C148:C149"/>
+    <mergeCell ref="C556:C557"/>
+    <mergeCell ref="B778:B785"/>
+    <mergeCell ref="B442:B449"/>
+    <mergeCell ref="C234:C235"/>
+    <mergeCell ref="C134:C135"/>
+    <mergeCell ref="C476:C477"/>
+    <mergeCell ref="C242:C243"/>
+    <mergeCell ref="C236:C237"/>
+    <mergeCell ref="C478:C479"/>
+    <mergeCell ref="C776:C777"/>
+    <mergeCell ref="C774:C775"/>
+    <mergeCell ref="C690:C691"/>
+    <mergeCell ref="C494:C495"/>
+    <mergeCell ref="C780:C781"/>
+    <mergeCell ref="C388:C389"/>
+    <mergeCell ref="C772:C773"/>
+    <mergeCell ref="C182:C183"/>
+    <mergeCell ref="B642:B649"/>
+    <mergeCell ref="B698:B705"/>
+    <mergeCell ref="B402:B409"/>
+    <mergeCell ref="B706:B713"/>
+    <mergeCell ref="C640:C641"/>
+    <mergeCell ref="C734:C735"/>
+    <mergeCell ref="B466:B473"/>
+    <mergeCell ref="C500:C501"/>
+    <mergeCell ref="C782:C783"/>
+    <mergeCell ref="B362:B369"/>
+    <mergeCell ref="C442:C443"/>
+    <mergeCell ref="C502:C503"/>
+    <mergeCell ref="B610:B617"/>
+    <mergeCell ref="C548:C549"/>
+    <mergeCell ref="C362:C363"/>
+    <mergeCell ref="C660:C661"/>
+    <mergeCell ref="B770:B777"/>
+    <mergeCell ref="C518:C519"/>
+    <mergeCell ref="C366:C367"/>
+    <mergeCell ref="C468:C469"/>
+    <mergeCell ref="B546:B553"/>
+    <mergeCell ref="C666:C667"/>
+    <mergeCell ref="C432:C433"/>
+    <mergeCell ref="B650:B657"/>
+    <mergeCell ref="B714:B721"/>
+    <mergeCell ref="C732:C733"/>
+    <mergeCell ref="C592:C593"/>
+    <mergeCell ref="C508:C509"/>
+    <mergeCell ref="B530:B537"/>
+    <mergeCell ref="C744:C745"/>
+    <mergeCell ref="C414:C415"/>
+    <mergeCell ref="C450:C451"/>
+    <mergeCell ref="B370:B377"/>
+    <mergeCell ref="C546:C547"/>
+    <mergeCell ref="C144:C145"/>
+    <mergeCell ref="C170:C171"/>
+    <mergeCell ref="B154:B161"/>
+    <mergeCell ref="C172:C173"/>
+    <mergeCell ref="C350:C351"/>
+    <mergeCell ref="C150:C151"/>
+    <mergeCell ref="C352:C353"/>
+    <mergeCell ref="C208:C209"/>
+    <mergeCell ref="B274:B281"/>
+    <mergeCell ref="C158:C159"/>
+    <mergeCell ref="B314:B321"/>
+    <mergeCell ref="B338:B345"/>
+    <mergeCell ref="C160:C161"/>
+    <mergeCell ref="C520:C521"/>
+    <mergeCell ref="C180:C181"/>
+    <mergeCell ref="C422:C423"/>
+    <mergeCell ref="C482:C483"/>
+    <mergeCell ref="C416:C417"/>
+    <mergeCell ref="C792:C793"/>
+    <mergeCell ref="C596:C597"/>
+    <mergeCell ref="C400:C401"/>
+    <mergeCell ref="A642:A721"/>
+    <mergeCell ref="B322:B329"/>
+    <mergeCell ref="C316:C317"/>
+    <mergeCell ref="C120:C121"/>
+    <mergeCell ref="C698:C699"/>
+    <mergeCell ref="C552:C553"/>
+    <mergeCell ref="C650:C651"/>
+    <mergeCell ref="C454:C455"/>
+    <mergeCell ref="C616:C617"/>
+    <mergeCell ref="C714:C715"/>
+    <mergeCell ref="C268:C269"/>
+    <mergeCell ref="B146:B153"/>
+    <mergeCell ref="C360:C361"/>
+    <mergeCell ref="B578:B585"/>
+    <mergeCell ref="C126:C127"/>
+    <mergeCell ref="B586:B593"/>
+    <mergeCell ref="C220:C221"/>
+    <mergeCell ref="C334:C335"/>
+    <mergeCell ref="C676:C677"/>
+    <mergeCell ref="C570:C571"/>
+    <mergeCell ref="C284:C285"/>
+    <mergeCell ref="C784:C785"/>
+    <mergeCell ref="C94:C95"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="C252:C253"/>
+    <mergeCell ref="C550:C551"/>
+    <mergeCell ref="C786:C787"/>
+    <mergeCell ref="B18:B25"/>
+    <mergeCell ref="C710:C711"/>
+    <mergeCell ref="C328:C329"/>
+    <mergeCell ref="C262:C263"/>
+    <mergeCell ref="C626:C627"/>
+    <mergeCell ref="C326:C327"/>
+    <mergeCell ref="C568:C569"/>
+    <mergeCell ref="C628:C629"/>
+    <mergeCell ref="C174:C175"/>
+    <mergeCell ref="C726:C727"/>
+    <mergeCell ref="C410:C411"/>
+    <mergeCell ref="B354:B361"/>
+    <mergeCell ref="C766:C767"/>
+    <mergeCell ref="B418:B425"/>
+    <mergeCell ref="B122:B129"/>
+    <mergeCell ref="C54:C55"/>
+    <mergeCell ref="C728:C729"/>
+    <mergeCell ref="C100:C101"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="C128:C129"/>
+    <mergeCell ref="C184:C185"/>
+    <mergeCell ref="C426:C427"/>
+    <mergeCell ref="C486:C487"/>
+    <mergeCell ref="C146:C147"/>
+    <mergeCell ref="C336:C337"/>
+    <mergeCell ref="C56:C57"/>
+    <mergeCell ref="C60:C61"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="C34:C35"/>
+    <mergeCell ref="C42:C43"/>
+    <mergeCell ref="C344:C345"/>
+    <mergeCell ref="C50:C51"/>
+    <mergeCell ref="C44:C45"/>
+    <mergeCell ref="C286:C287"/>
+    <mergeCell ref="C36:C37"/>
+    <mergeCell ref="C48:C49"/>
+    <mergeCell ref="C346:C347"/>
+    <mergeCell ref="C130:C131"/>
+    <mergeCell ref="C72:C73"/>
+    <mergeCell ref="C124:C125"/>
+    <mergeCell ref="C118:C119"/>
+    <mergeCell ref="C90:C91"/>
+    <mergeCell ref="A2:A81"/>
+    <mergeCell ref="B498:B505"/>
+    <mergeCell ref="B114:B121"/>
+    <mergeCell ref="C338:C339"/>
+    <mergeCell ref="C104:C105"/>
+    <mergeCell ref="C536:C537"/>
+    <mergeCell ref="C340:C341"/>
+    <mergeCell ref="C196:C197"/>
+    <mergeCell ref="B66:B73"/>
+    <mergeCell ref="C302:C303"/>
+    <mergeCell ref="C404:C405"/>
+    <mergeCell ref="B522:B529"/>
+    <mergeCell ref="C394:C395"/>
+    <mergeCell ref="C198:C199"/>
+    <mergeCell ref="B130:B137"/>
+    <mergeCell ref="C458:C459"/>
+    <mergeCell ref="C110:C111"/>
+    <mergeCell ref="C408:C409"/>
+    <mergeCell ref="B290:B297"/>
+    <mergeCell ref="B346:B353"/>
+    <mergeCell ref="A402:A481"/>
+    <mergeCell ref="B394:B401"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="C186:C187"/>
+    <mergeCell ref="C664:C665"/>
+    <mergeCell ref="C694:C695"/>
+    <mergeCell ref="C758:C759"/>
+    <mergeCell ref="C484:C485"/>
+    <mergeCell ref="C384:C385"/>
+    <mergeCell ref="C142:C143"/>
+    <mergeCell ref="C584:C585"/>
+    <mergeCell ref="C80:C81"/>
+    <mergeCell ref="C106:C107"/>
+    <mergeCell ref="C748:C749"/>
+    <mergeCell ref="C436:C437"/>
+    <mergeCell ref="C380:C381"/>
+    <mergeCell ref="C224:C225"/>
+    <mergeCell ref="C742:C743"/>
+    <mergeCell ref="C736:C737"/>
+    <mergeCell ref="C572:C573"/>
+    <mergeCell ref="C686:C687"/>
+    <mergeCell ref="C574:C575"/>
+    <mergeCell ref="C720:C721"/>
+    <mergeCell ref="C642:C643"/>
+    <mergeCell ref="C678:C679"/>
+    <mergeCell ref="C674:C675"/>
+    <mergeCell ref="B754:B761"/>
+    <mergeCell ref="C386:C387"/>
+    <mergeCell ref="B554:B561"/>
+    <mergeCell ref="C594:C595"/>
+    <mergeCell ref="C246:C247"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="C612:C613"/>
+    <mergeCell ref="C704:C705"/>
+    <mergeCell ref="C176:C177"/>
+    <mergeCell ref="C418:C419"/>
+    <mergeCell ref="C356:C357"/>
+    <mergeCell ref="C70:C71"/>
+    <mergeCell ref="C412:C413"/>
+    <mergeCell ref="C312:C313"/>
+    <mergeCell ref="C610:C611"/>
+    <mergeCell ref="C470:C471"/>
+    <mergeCell ref="B162:B169"/>
+    <mergeCell ref="C38:C39"/>
+    <mergeCell ref="B562:B569"/>
+    <mergeCell ref="B626:B633"/>
+    <mergeCell ref="B738:B745"/>
+    <mergeCell ref="C52:C53"/>
+    <mergeCell ref="B378:B385"/>
+    <mergeCell ref="C62:C63"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="C304:C305"/>
+    <mergeCell ref="C480:C481"/>
+    <mergeCell ref="C98:C99"/>
+    <mergeCell ref="C540:C541"/>
+    <mergeCell ref="C602:C603"/>
+    <mergeCell ref="C396:C397"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="C368:C369"/>
+    <mergeCell ref="C306:C307"/>
+    <mergeCell ref="C162:C163"/>
+    <mergeCell ref="C460:C461"/>
+    <mergeCell ref="C398:C399"/>
+    <mergeCell ref="C112:C113"/>
+    <mergeCell ref="C364:C365"/>
+    <mergeCell ref="C152:C153"/>
+    <mergeCell ref="C462:C463"/>
+    <mergeCell ref="C82:C83"/>
+    <mergeCell ref="C292:C293"/>
+    <mergeCell ref="C534:C535"/>
+    <mergeCell ref="C528:C529"/>
+    <mergeCell ref="C586:C587"/>
+    <mergeCell ref="C58:C59"/>
+    <mergeCell ref="C294:C295"/>
+    <mergeCell ref="B794:B801"/>
+    <mergeCell ref="C228:C229"/>
+    <mergeCell ref="C222:C223"/>
+    <mergeCell ref="C526:C527"/>
+    <mergeCell ref="B682:B689"/>
+    <mergeCell ref="C762:C763"/>
+    <mergeCell ref="B538:B545"/>
+    <mergeCell ref="C578:C579"/>
+    <mergeCell ref="C86:C87"/>
+    <mergeCell ref="B746:B753"/>
+    <mergeCell ref="B602:B609"/>
+    <mergeCell ref="C538:C539"/>
+    <mergeCell ref="B306:B313"/>
+    <mergeCell ref="C604:C605"/>
+    <mergeCell ref="C702:C703"/>
+    <mergeCell ref="C696:C697"/>
+    <mergeCell ref="B330:B337"/>
+    <mergeCell ref="C668:C669"/>
+    <mergeCell ref="C760:C761"/>
+    <mergeCell ref="B98:B105"/>
+    <mergeCell ref="C622:C623"/>
+    <mergeCell ref="B250:B257"/>
+    <mergeCell ref="B490:B497"/>
+    <mergeCell ref="C392:C393"/>
+    <mergeCell ref="B26:B33"/>
+    <mergeCell ref="C250:C251"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="C654:C655"/>
+    <mergeCell ref="C510:C511"/>
+    <mergeCell ref="B90:B97"/>
+    <mergeCell ref="C752:C753"/>
+    <mergeCell ref="C276:C277"/>
+    <mergeCell ref="C214:C215"/>
+    <mergeCell ref="C512:C513"/>
+    <mergeCell ref="C226:C227"/>
+    <mergeCell ref="C164:C165"/>
+    <mergeCell ref="B42:B49"/>
+    <mergeCell ref="C278:C279"/>
+    <mergeCell ref="C576:C577"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="C342:C343"/>
+    <mergeCell ref="C136:C137"/>
+    <mergeCell ref="B258:B265"/>
+    <mergeCell ref="C434:C435"/>
+    <mergeCell ref="C670:C671"/>
+    <mergeCell ref="C390:C391"/>
+    <mergeCell ref="C200:C201"/>
+    <mergeCell ref="B266:B273"/>
+    <mergeCell ref="B10:B17"/>
+    <mergeCell ref="C636:C637"/>
+    <mergeCell ref="B658:B665"/>
+    <mergeCell ref="B58:B65"/>
+    <mergeCell ref="C138:C139"/>
+    <mergeCell ref="C76:C77"/>
+    <mergeCell ref="C580:C581"/>
+    <mergeCell ref="C632:C633"/>
+    <mergeCell ref="C140:C141"/>
+    <mergeCell ref="C582:C583"/>
+    <mergeCell ref="C438:C439"/>
+    <mergeCell ref="B594:B601"/>
+    <mergeCell ref="C620:C621"/>
+    <mergeCell ref="C504:C505"/>
+    <mergeCell ref="B138:B145"/>
+    <mergeCell ref="C156:C157"/>
+    <mergeCell ref="C506:C507"/>
+    <mergeCell ref="C522:C523"/>
+    <mergeCell ref="C354:C355"/>
+    <mergeCell ref="C288:C289"/>
+    <mergeCell ref="C348:C349"/>
+    <mergeCell ref="C652:C653"/>
+    <mergeCell ref="C204:C205"/>
+    <mergeCell ref="C590:C591"/>
+    <mergeCell ref="B386:B393"/>
+    <mergeCell ref="C562:C563"/>
+    <mergeCell ref="B242:B249"/>
+    <mergeCell ref="C662:C663"/>
+    <mergeCell ref="C270:C271"/>
+    <mergeCell ref="B450:B457"/>
+    <mergeCell ref="C46:C47"/>
+    <mergeCell ref="C40:C41"/>
+    <mergeCell ref="C282:C283"/>
+    <mergeCell ref="B74:B81"/>
+    <mergeCell ref="C154:C155"/>
+    <mergeCell ref="C212:C213"/>
+    <mergeCell ref="C206:C207"/>
+    <mergeCell ref="C648:C649"/>
+    <mergeCell ref="C448:C449"/>
+    <mergeCell ref="C446:C447"/>
+    <mergeCell ref="C646:C647"/>
+    <mergeCell ref="C440:C441"/>
+    <mergeCell ref="C232:C233"/>
+    <mergeCell ref="C530:C531"/>
+    <mergeCell ref="C430:C431"/>
+    <mergeCell ref="C588:C589"/>
+    <mergeCell ref="C122:C123"/>
+    <mergeCell ref="C178:C179"/>
+    <mergeCell ref="C496:C497"/>
+    <mergeCell ref="C794:C795"/>
+    <mergeCell ref="C216:C217"/>
+    <mergeCell ref="C514:C515"/>
+    <mergeCell ref="C452:C453"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="C750:C751"/>
+    <mergeCell ref="C318:C319"/>
+    <mergeCell ref="C560:C561"/>
+    <mergeCell ref="C280:C281"/>
+    <mergeCell ref="C516:C517"/>
+    <mergeCell ref="C84:C85"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="C320:C321"/>
+    <mergeCell ref="C680:C681"/>
+    <mergeCell ref="C768:C769"/>
+    <mergeCell ref="C78:C79"/>
+    <mergeCell ref="C420:C421"/>
+    <mergeCell ref="C376:C377"/>
+    <mergeCell ref="C718:C719"/>
+    <mergeCell ref="C314:C315"/>
+    <mergeCell ref="C770:C771"/>
+    <mergeCell ref="C600:C601"/>
+    <mergeCell ref="C692:C693"/>
     <mergeCell ref="B2:B9"/>
     <mergeCell ref="C188:C189"/>
     <mergeCell ref="C424:C425"/>
@@ -54100,469 +54551,30 @@
     <mergeCell ref="C330:C331"/>
     <mergeCell ref="B282:B289"/>
     <mergeCell ref="C566:C567"/>
+    <mergeCell ref="C800:C801"/>
+    <mergeCell ref="C210:C211"/>
+    <mergeCell ref="C324:C325"/>
+    <mergeCell ref="B194:B201"/>
+    <mergeCell ref="C274:C275"/>
+    <mergeCell ref="B50:B57"/>
+    <mergeCell ref="C114:C115"/>
+    <mergeCell ref="B690:B697"/>
+    <mergeCell ref="C132:C133"/>
+    <mergeCell ref="C272:C273"/>
+    <mergeCell ref="C332:C333"/>
+    <mergeCell ref="C630:C631"/>
+    <mergeCell ref="C778:C779"/>
+    <mergeCell ref="C796:C797"/>
+    <mergeCell ref="C682:C683"/>
+    <mergeCell ref="C738:C739"/>
+    <mergeCell ref="B666:B673"/>
+    <mergeCell ref="C746:C747"/>
+    <mergeCell ref="B730:B737"/>
+    <mergeCell ref="B674:B681"/>
+    <mergeCell ref="C370:C371"/>
+    <mergeCell ref="C96:C97"/>
+    <mergeCell ref="C532:C533"/>
     <mergeCell ref="B722:B729"/>
-    <mergeCell ref="C496:C497"/>
-    <mergeCell ref="C794:C795"/>
-    <mergeCell ref="C216:C217"/>
-    <mergeCell ref="C514:C515"/>
-    <mergeCell ref="C452:C453"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="C750:C751"/>
-    <mergeCell ref="C318:C319"/>
-    <mergeCell ref="C560:C561"/>
-    <mergeCell ref="C280:C281"/>
-    <mergeCell ref="C516:C517"/>
-    <mergeCell ref="C84:C85"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="C320:C321"/>
-    <mergeCell ref="B386:B393"/>
-    <mergeCell ref="C562:C563"/>
-    <mergeCell ref="B242:B249"/>
-    <mergeCell ref="C662:C663"/>
-    <mergeCell ref="C270:C271"/>
-    <mergeCell ref="B450:B457"/>
-    <mergeCell ref="C46:C47"/>
-    <mergeCell ref="C40:C41"/>
-    <mergeCell ref="C282:C283"/>
-    <mergeCell ref="B74:B81"/>
-    <mergeCell ref="C154:C155"/>
-    <mergeCell ref="C212:C213"/>
-    <mergeCell ref="C206:C207"/>
-    <mergeCell ref="C648:C649"/>
-    <mergeCell ref="C448:C449"/>
-    <mergeCell ref="B10:B17"/>
-    <mergeCell ref="C636:C637"/>
-    <mergeCell ref="B658:B665"/>
-    <mergeCell ref="B58:B65"/>
-    <mergeCell ref="C138:C139"/>
-    <mergeCell ref="C76:C77"/>
-    <mergeCell ref="C580:C581"/>
-    <mergeCell ref="C632:C633"/>
-    <mergeCell ref="C140:C141"/>
-    <mergeCell ref="C582:C583"/>
-    <mergeCell ref="C438:C439"/>
-    <mergeCell ref="B594:B601"/>
-    <mergeCell ref="C620:C621"/>
-    <mergeCell ref="C504:C505"/>
-    <mergeCell ref="B138:B145"/>
-    <mergeCell ref="C156:C157"/>
-    <mergeCell ref="C506:C507"/>
-    <mergeCell ref="C522:C523"/>
-    <mergeCell ref="C680:C681"/>
-    <mergeCell ref="C354:C355"/>
-    <mergeCell ref="C288:C289"/>
-    <mergeCell ref="C348:C349"/>
-    <mergeCell ref="C652:C653"/>
-    <mergeCell ref="C204:C205"/>
-    <mergeCell ref="C590:C591"/>
-    <mergeCell ref="C446:C447"/>
-    <mergeCell ref="C646:C647"/>
-    <mergeCell ref="C440:C441"/>
-    <mergeCell ref="C232:C233"/>
-    <mergeCell ref="C530:C531"/>
-    <mergeCell ref="C430:C431"/>
-    <mergeCell ref="C588:C589"/>
-    <mergeCell ref="B26:B33"/>
-    <mergeCell ref="C250:C251"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="C654:C655"/>
-    <mergeCell ref="C510:C511"/>
-    <mergeCell ref="B90:B97"/>
-    <mergeCell ref="C752:C753"/>
-    <mergeCell ref="C276:C277"/>
-    <mergeCell ref="C214:C215"/>
-    <mergeCell ref="C512:C513"/>
-    <mergeCell ref="C226:C227"/>
-    <mergeCell ref="C164:C165"/>
-    <mergeCell ref="B42:B49"/>
-    <mergeCell ref="C278:C279"/>
-    <mergeCell ref="C576:C577"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="C342:C343"/>
-    <mergeCell ref="C136:C137"/>
-    <mergeCell ref="B258:B265"/>
-    <mergeCell ref="C434:C435"/>
-    <mergeCell ref="C670:C671"/>
-    <mergeCell ref="C390:C391"/>
-    <mergeCell ref="C200:C201"/>
-    <mergeCell ref="B266:B273"/>
-    <mergeCell ref="B794:B801"/>
-    <mergeCell ref="C228:C229"/>
-    <mergeCell ref="C222:C223"/>
-    <mergeCell ref="C526:C527"/>
-    <mergeCell ref="B682:B689"/>
-    <mergeCell ref="C762:C763"/>
-    <mergeCell ref="B538:B545"/>
-    <mergeCell ref="C578:C579"/>
-    <mergeCell ref="C86:C87"/>
-    <mergeCell ref="B746:B753"/>
-    <mergeCell ref="B602:B609"/>
-    <mergeCell ref="C538:C539"/>
-    <mergeCell ref="B306:B313"/>
-    <mergeCell ref="C604:C605"/>
-    <mergeCell ref="C702:C703"/>
-    <mergeCell ref="C696:C697"/>
-    <mergeCell ref="B330:B337"/>
-    <mergeCell ref="C668:C669"/>
-    <mergeCell ref="C760:C761"/>
-    <mergeCell ref="B98:B105"/>
-    <mergeCell ref="C622:C623"/>
-    <mergeCell ref="B250:B257"/>
-    <mergeCell ref="B490:B497"/>
-    <mergeCell ref="C392:C393"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="C304:C305"/>
-    <mergeCell ref="C480:C481"/>
-    <mergeCell ref="C98:C99"/>
-    <mergeCell ref="C540:C541"/>
-    <mergeCell ref="C602:C603"/>
-    <mergeCell ref="C396:C397"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="C368:C369"/>
-    <mergeCell ref="C306:C307"/>
-    <mergeCell ref="C162:C163"/>
-    <mergeCell ref="C460:C461"/>
-    <mergeCell ref="C398:C399"/>
-    <mergeCell ref="C112:C113"/>
-    <mergeCell ref="C364:C365"/>
-    <mergeCell ref="C152:C153"/>
-    <mergeCell ref="C462:C463"/>
-    <mergeCell ref="C82:C83"/>
-    <mergeCell ref="C292:C293"/>
-    <mergeCell ref="C534:C535"/>
-    <mergeCell ref="C528:C529"/>
-    <mergeCell ref="C586:C587"/>
-    <mergeCell ref="C58:C59"/>
-    <mergeCell ref="C294:C295"/>
-    <mergeCell ref="B754:B761"/>
-    <mergeCell ref="C386:C387"/>
-    <mergeCell ref="B554:B561"/>
-    <mergeCell ref="C594:C595"/>
-    <mergeCell ref="C246:C247"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="C612:C613"/>
-    <mergeCell ref="C704:C705"/>
-    <mergeCell ref="C176:C177"/>
-    <mergeCell ref="C418:C419"/>
-    <mergeCell ref="C356:C357"/>
-    <mergeCell ref="C70:C71"/>
-    <mergeCell ref="C412:C413"/>
-    <mergeCell ref="C312:C313"/>
-    <mergeCell ref="C610:C611"/>
-    <mergeCell ref="C470:C471"/>
-    <mergeCell ref="B162:B169"/>
-    <mergeCell ref="C38:C39"/>
-    <mergeCell ref="B562:B569"/>
-    <mergeCell ref="B626:B633"/>
-    <mergeCell ref="B738:B745"/>
-    <mergeCell ref="C52:C53"/>
-    <mergeCell ref="B378:B385"/>
-    <mergeCell ref="C62:C63"/>
-    <mergeCell ref="C768:C769"/>
-    <mergeCell ref="C122:C123"/>
-    <mergeCell ref="C178:C179"/>
-    <mergeCell ref="C78:C79"/>
-    <mergeCell ref="C420:C421"/>
-    <mergeCell ref="C376:C377"/>
-    <mergeCell ref="C718:C719"/>
-    <mergeCell ref="C314:C315"/>
-    <mergeCell ref="C770:C771"/>
-    <mergeCell ref="C600:C601"/>
-    <mergeCell ref="C692:C693"/>
-    <mergeCell ref="C664:C665"/>
-    <mergeCell ref="C694:C695"/>
-    <mergeCell ref="C758:C759"/>
-    <mergeCell ref="C484:C485"/>
-    <mergeCell ref="C384:C385"/>
-    <mergeCell ref="C142:C143"/>
-    <mergeCell ref="C584:C585"/>
-    <mergeCell ref="C80:C81"/>
-    <mergeCell ref="C106:C107"/>
-    <mergeCell ref="C748:C749"/>
-    <mergeCell ref="C436:C437"/>
-    <mergeCell ref="C380:C381"/>
-    <mergeCell ref="C224:C225"/>
-    <mergeCell ref="A2:A81"/>
-    <mergeCell ref="B498:B505"/>
-    <mergeCell ref="B114:B121"/>
-    <mergeCell ref="C338:C339"/>
-    <mergeCell ref="C104:C105"/>
-    <mergeCell ref="C536:C537"/>
-    <mergeCell ref="C340:C341"/>
-    <mergeCell ref="C196:C197"/>
-    <mergeCell ref="B66:B73"/>
-    <mergeCell ref="C302:C303"/>
-    <mergeCell ref="C404:C405"/>
-    <mergeCell ref="B522:B529"/>
-    <mergeCell ref="C394:C395"/>
-    <mergeCell ref="C198:C199"/>
-    <mergeCell ref="B130:B137"/>
-    <mergeCell ref="C458:C459"/>
-    <mergeCell ref="C110:C111"/>
-    <mergeCell ref="C408:C409"/>
-    <mergeCell ref="B290:B297"/>
-    <mergeCell ref="B346:B353"/>
-    <mergeCell ref="A402:A481"/>
-    <mergeCell ref="B394:B401"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="C186:C187"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="C128:C129"/>
-    <mergeCell ref="C184:C185"/>
-    <mergeCell ref="C426:C427"/>
-    <mergeCell ref="C486:C487"/>
-    <mergeCell ref="C146:C147"/>
-    <mergeCell ref="C336:C337"/>
-    <mergeCell ref="C56:C57"/>
-    <mergeCell ref="C60:C61"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="C34:C35"/>
-    <mergeCell ref="C42:C43"/>
-    <mergeCell ref="C344:C345"/>
-    <mergeCell ref="C50:C51"/>
-    <mergeCell ref="C44:C45"/>
-    <mergeCell ref="C286:C287"/>
-    <mergeCell ref="C36:C37"/>
-    <mergeCell ref="C48:C49"/>
-    <mergeCell ref="C346:C347"/>
-    <mergeCell ref="C130:C131"/>
-    <mergeCell ref="C72:C73"/>
-    <mergeCell ref="C784:C785"/>
-    <mergeCell ref="C94:C95"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="C252:C253"/>
-    <mergeCell ref="C550:C551"/>
-    <mergeCell ref="C786:C787"/>
-    <mergeCell ref="B18:B25"/>
-    <mergeCell ref="C710:C711"/>
-    <mergeCell ref="C328:C329"/>
-    <mergeCell ref="C262:C263"/>
-    <mergeCell ref="C626:C627"/>
-    <mergeCell ref="C326:C327"/>
-    <mergeCell ref="C568:C569"/>
-    <mergeCell ref="C628:C629"/>
-    <mergeCell ref="C174:C175"/>
-    <mergeCell ref="C726:C727"/>
-    <mergeCell ref="C410:C411"/>
-    <mergeCell ref="B354:B361"/>
-    <mergeCell ref="C766:C767"/>
-    <mergeCell ref="B418:B425"/>
-    <mergeCell ref="B122:B129"/>
-    <mergeCell ref="C54:C55"/>
-    <mergeCell ref="C728:C729"/>
-    <mergeCell ref="C100:C101"/>
-    <mergeCell ref="C792:C793"/>
-    <mergeCell ref="C596:C597"/>
-    <mergeCell ref="C400:C401"/>
-    <mergeCell ref="A642:A721"/>
-    <mergeCell ref="B322:B329"/>
-    <mergeCell ref="C316:C317"/>
-    <mergeCell ref="C120:C121"/>
-    <mergeCell ref="C698:C699"/>
-    <mergeCell ref="C552:C553"/>
-    <mergeCell ref="C650:C651"/>
-    <mergeCell ref="C454:C455"/>
-    <mergeCell ref="C616:C617"/>
-    <mergeCell ref="C714:C715"/>
-    <mergeCell ref="C268:C269"/>
-    <mergeCell ref="B146:B153"/>
-    <mergeCell ref="C360:C361"/>
-    <mergeCell ref="B578:B585"/>
-    <mergeCell ref="C126:C127"/>
-    <mergeCell ref="B586:B593"/>
-    <mergeCell ref="C220:C221"/>
-    <mergeCell ref="C334:C335"/>
-    <mergeCell ref="C676:C677"/>
-    <mergeCell ref="C570:C571"/>
-    <mergeCell ref="C284:C285"/>
-    <mergeCell ref="C742:C743"/>
-    <mergeCell ref="C736:C737"/>
-    <mergeCell ref="B370:B377"/>
-    <mergeCell ref="C546:C547"/>
-    <mergeCell ref="C144:C145"/>
-    <mergeCell ref="C170:C171"/>
-    <mergeCell ref="B154:B161"/>
-    <mergeCell ref="C172:C173"/>
-    <mergeCell ref="C350:C351"/>
-    <mergeCell ref="C150:C151"/>
-    <mergeCell ref="C352:C353"/>
-    <mergeCell ref="C208:C209"/>
-    <mergeCell ref="B274:B281"/>
-    <mergeCell ref="C572:C573"/>
-    <mergeCell ref="C686:C687"/>
-    <mergeCell ref="C158:C159"/>
-    <mergeCell ref="B314:B321"/>
-    <mergeCell ref="B338:B345"/>
-    <mergeCell ref="C574:C575"/>
-    <mergeCell ref="C160:C161"/>
-    <mergeCell ref="C720:C721"/>
-    <mergeCell ref="C520:C521"/>
-    <mergeCell ref="C642:C643"/>
-    <mergeCell ref="C678:C679"/>
-    <mergeCell ref="C782:C783"/>
-    <mergeCell ref="B362:B369"/>
-    <mergeCell ref="C442:C443"/>
-    <mergeCell ref="C502:C503"/>
-    <mergeCell ref="B610:B617"/>
-    <mergeCell ref="C548:C549"/>
-    <mergeCell ref="C362:C363"/>
-    <mergeCell ref="C660:C661"/>
-    <mergeCell ref="B770:B777"/>
-    <mergeCell ref="C518:C519"/>
-    <mergeCell ref="C366:C367"/>
-    <mergeCell ref="C468:C469"/>
-    <mergeCell ref="B546:B553"/>
-    <mergeCell ref="C666:C667"/>
-    <mergeCell ref="C432:C433"/>
-    <mergeCell ref="B650:B657"/>
-    <mergeCell ref="B714:B721"/>
-    <mergeCell ref="C732:C733"/>
-    <mergeCell ref="C592:C593"/>
-    <mergeCell ref="C508:C509"/>
-    <mergeCell ref="B530:B537"/>
-    <mergeCell ref="C744:C745"/>
-    <mergeCell ref="C414:C415"/>
-    <mergeCell ref="C450:C451"/>
-    <mergeCell ref="B778:B785"/>
-    <mergeCell ref="B442:B449"/>
-    <mergeCell ref="C234:C235"/>
-    <mergeCell ref="C134:C135"/>
-    <mergeCell ref="C476:C477"/>
-    <mergeCell ref="C242:C243"/>
-    <mergeCell ref="C236:C237"/>
-    <mergeCell ref="C478:C479"/>
-    <mergeCell ref="C776:C777"/>
-    <mergeCell ref="C774:C775"/>
-    <mergeCell ref="C690:C691"/>
-    <mergeCell ref="C494:C495"/>
-    <mergeCell ref="C780:C781"/>
-    <mergeCell ref="C388:C389"/>
-    <mergeCell ref="C772:C773"/>
-    <mergeCell ref="C182:C183"/>
-    <mergeCell ref="B642:B649"/>
-    <mergeCell ref="B698:B705"/>
-    <mergeCell ref="B402:B409"/>
-    <mergeCell ref="B706:B713"/>
-    <mergeCell ref="C640:C641"/>
-    <mergeCell ref="C734:C735"/>
-    <mergeCell ref="B466:B473"/>
-    <mergeCell ref="C500:C501"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="C300:C301"/>
-    <mergeCell ref="C66:C67"/>
-    <mergeCell ref="C498:C499"/>
-    <mergeCell ref="C740:C741"/>
-    <mergeCell ref="B762:B769"/>
-    <mergeCell ref="B234:B241"/>
-    <mergeCell ref="B618:B625"/>
-    <mergeCell ref="C264:C265"/>
-    <mergeCell ref="B186:B193"/>
-    <mergeCell ref="C358:C359"/>
-    <mergeCell ref="C656:C657"/>
-    <mergeCell ref="C618:C619"/>
-    <mergeCell ref="C658:C659"/>
-    <mergeCell ref="C756:C757"/>
-    <mergeCell ref="C378:C379"/>
-    <mergeCell ref="C166:C167"/>
-    <mergeCell ref="C464:C465"/>
-    <mergeCell ref="C402:C403"/>
-    <mergeCell ref="C524:C525"/>
-    <mergeCell ref="C712:C713"/>
-    <mergeCell ref="B106:B113"/>
-    <mergeCell ref="C148:C149"/>
-    <mergeCell ref="C556:C557"/>
-    <mergeCell ref="B786:B793"/>
-    <mergeCell ref="C218:C219"/>
-    <mergeCell ref="C638:C639"/>
-    <mergeCell ref="C230:C231"/>
-    <mergeCell ref="C168:C169"/>
-    <mergeCell ref="C290:C291"/>
-    <mergeCell ref="C466:C467"/>
-    <mergeCell ref="C764:C765"/>
-    <mergeCell ref="C382:C383"/>
-    <mergeCell ref="C624:C625"/>
-    <mergeCell ref="B170:B177"/>
-    <mergeCell ref="C688:C689"/>
-    <mergeCell ref="C684:C685"/>
-    <mergeCell ref="C192:C193"/>
-    <mergeCell ref="C428:C429"/>
-    <mergeCell ref="C238:C239"/>
-    <mergeCell ref="C474:C475"/>
-    <mergeCell ref="C194:C195"/>
-    <mergeCell ref="C492:C493"/>
-    <mergeCell ref="C240:C241"/>
-    <mergeCell ref="C296:C297"/>
-    <mergeCell ref="C598:C599"/>
-    <mergeCell ref="B178:B185"/>
-    <mergeCell ref="C258:C259"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="C244:C245"/>
-    <mergeCell ref="C542:C543"/>
-    <mergeCell ref="C700:C701"/>
-    <mergeCell ref="C308:C309"/>
-    <mergeCell ref="C606:C607"/>
-    <mergeCell ref="C102:C103"/>
-    <mergeCell ref="C544:C545"/>
-    <mergeCell ref="B34:B41"/>
-    <mergeCell ref="C564:C565"/>
-    <mergeCell ref="C74:C75"/>
-    <mergeCell ref="C68:C69"/>
-    <mergeCell ref="C372:C373"/>
-    <mergeCell ref="C310:C311"/>
-    <mergeCell ref="B506:B513"/>
-    <mergeCell ref="C608:C609"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="C116:C117"/>
-    <mergeCell ref="B570:B577"/>
-    <mergeCell ref="B458:B465"/>
-    <mergeCell ref="B634:B641"/>
-    <mergeCell ref="B202:B209"/>
-    <mergeCell ref="C202:C203"/>
-    <mergeCell ref="C444:C445"/>
-    <mergeCell ref="C124:C125"/>
-    <mergeCell ref="C180:C181"/>
-    <mergeCell ref="C118:C119"/>
-    <mergeCell ref="C422:C423"/>
-    <mergeCell ref="C482:C483"/>
-    <mergeCell ref="C416:C417"/>
-    <mergeCell ref="C674:C675"/>
-    <mergeCell ref="C90:C91"/>
-    <mergeCell ref="A82:A161"/>
-    <mergeCell ref="A562:A641"/>
-    <mergeCell ref="A482:A561"/>
-    <mergeCell ref="C644:C645"/>
-    <mergeCell ref="A242:A321"/>
-    <mergeCell ref="C92:C93"/>
-    <mergeCell ref="B82:B89"/>
-    <mergeCell ref="C634:C635"/>
-    <mergeCell ref="B210:B217"/>
-    <mergeCell ref="B514:B521"/>
-    <mergeCell ref="B298:B305"/>
-    <mergeCell ref="A322:A401"/>
-    <mergeCell ref="C798:C799"/>
-    <mergeCell ref="C108:C109"/>
-    <mergeCell ref="B226:B233"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="C266:C267"/>
-    <mergeCell ref="C322:C323"/>
-    <mergeCell ref="C260:C261"/>
-    <mergeCell ref="C558:C559"/>
-    <mergeCell ref="A162:A241"/>
-    <mergeCell ref="B426:B433"/>
-    <mergeCell ref="C298:C299"/>
-    <mergeCell ref="C456:C457"/>
-    <mergeCell ref="C754:C755"/>
-    <mergeCell ref="C64:C65"/>
-    <mergeCell ref="C406:C407"/>
-    <mergeCell ref="C614:C615"/>
-    <mergeCell ref="B482:B489"/>
-    <mergeCell ref="C706:C707"/>
-    <mergeCell ref="C374:C375"/>
-    <mergeCell ref="C716:C717"/>
-    <mergeCell ref="C672:C673"/>
-    <mergeCell ref="C88:C89"/>
-    <mergeCell ref="C472:C473"/>
-    <mergeCell ref="C708:C709"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -72045,6 +72057,92 @@
     </row>
   </sheetData>
   <mergeCells count="110">
+    <mergeCell ref="B398:B401"/>
+    <mergeCell ref="A362:A401"/>
+    <mergeCell ref="B222:B225"/>
+    <mergeCell ref="B114:B117"/>
+    <mergeCell ref="B154:B157"/>
+    <mergeCell ref="B206:B209"/>
+    <mergeCell ref="B390:B393"/>
+    <mergeCell ref="B138:B141"/>
+    <mergeCell ref="B374:B377"/>
+    <mergeCell ref="A162:A201"/>
+    <mergeCell ref="B386:B389"/>
+    <mergeCell ref="B190:B193"/>
+    <mergeCell ref="B322:B325"/>
+    <mergeCell ref="B262:B265"/>
+    <mergeCell ref="B86:B89"/>
+    <mergeCell ref="B370:B373"/>
+    <mergeCell ref="B62:B65"/>
+    <mergeCell ref="B14:B17"/>
+    <mergeCell ref="B70:B73"/>
+    <mergeCell ref="B290:B293"/>
+    <mergeCell ref="A42:A81"/>
+    <mergeCell ref="B182:B185"/>
+    <mergeCell ref="B362:B365"/>
+    <mergeCell ref="B346:B349"/>
+    <mergeCell ref="B246:B249"/>
+    <mergeCell ref="A202:A241"/>
+    <mergeCell ref="B298:B301"/>
+    <mergeCell ref="A122:A161"/>
+    <mergeCell ref="B82:B85"/>
+    <mergeCell ref="B210:B213"/>
+    <mergeCell ref="B358:B361"/>
+    <mergeCell ref="B354:B357"/>
+    <mergeCell ref="B330:B333"/>
+    <mergeCell ref="B282:B285"/>
+    <mergeCell ref="B94:B97"/>
+    <mergeCell ref="B46:B49"/>
+    <mergeCell ref="B102:B105"/>
+    <mergeCell ref="B242:B245"/>
+    <mergeCell ref="B10:B13"/>
+    <mergeCell ref="B250:B253"/>
+    <mergeCell ref="B342:B345"/>
+    <mergeCell ref="B146:B149"/>
+    <mergeCell ref="B178:B181"/>
+    <mergeCell ref="B34:B37"/>
+    <mergeCell ref="B74:B77"/>
+    <mergeCell ref="A82:A121"/>
+    <mergeCell ref="B270:B273"/>
+    <mergeCell ref="B310:B313"/>
+    <mergeCell ref="B162:B165"/>
+    <mergeCell ref="B334:B337"/>
+    <mergeCell ref="B22:B25"/>
+    <mergeCell ref="B150:B153"/>
+    <mergeCell ref="B326:B329"/>
+    <mergeCell ref="B254:B257"/>
+    <mergeCell ref="B30:B33"/>
+    <mergeCell ref="B198:B201"/>
+    <mergeCell ref="B174:B177"/>
+    <mergeCell ref="B126:B129"/>
+    <mergeCell ref="B218:B221"/>
+    <mergeCell ref="B110:B113"/>
+    <mergeCell ref="B54:B57"/>
+    <mergeCell ref="B202:B205"/>
+    <mergeCell ref="B98:B101"/>
+    <mergeCell ref="B394:B397"/>
+    <mergeCell ref="B338:B341"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="B186:B189"/>
+    <mergeCell ref="B230:B233"/>
+    <mergeCell ref="B142:B145"/>
+    <mergeCell ref="B226:B229"/>
+    <mergeCell ref="B266:B269"/>
+    <mergeCell ref="B378:B381"/>
+    <mergeCell ref="B306:B309"/>
+    <mergeCell ref="B26:B29"/>
+    <mergeCell ref="B134:B137"/>
+    <mergeCell ref="B194:B197"/>
+    <mergeCell ref="B90:B93"/>
+    <mergeCell ref="B122:B125"/>
+    <mergeCell ref="B214:B217"/>
+    <mergeCell ref="B18:B21"/>
+    <mergeCell ref="B294:B297"/>
+    <mergeCell ref="B106:B109"/>
+    <mergeCell ref="B382:B385"/>
+    <mergeCell ref="B42:B45"/>
+    <mergeCell ref="B278:B281"/>
+    <mergeCell ref="B170:B173"/>
     <mergeCell ref="B66:B69"/>
     <mergeCell ref="A242:A281"/>
     <mergeCell ref="B302:B305"/>
@@ -72069,92 +72167,6 @@
     <mergeCell ref="A322:A361"/>
     <mergeCell ref="B58:B61"/>
     <mergeCell ref="B234:B237"/>
-    <mergeCell ref="B98:B101"/>
-    <mergeCell ref="B394:B397"/>
-    <mergeCell ref="B338:B341"/>
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="B186:B189"/>
-    <mergeCell ref="B230:B233"/>
-    <mergeCell ref="B142:B145"/>
-    <mergeCell ref="B226:B229"/>
-    <mergeCell ref="B266:B269"/>
-    <mergeCell ref="B378:B381"/>
-    <mergeCell ref="B306:B309"/>
-    <mergeCell ref="B26:B29"/>
-    <mergeCell ref="B134:B137"/>
-    <mergeCell ref="B194:B197"/>
-    <mergeCell ref="B90:B93"/>
-    <mergeCell ref="B122:B125"/>
-    <mergeCell ref="B214:B217"/>
-    <mergeCell ref="B18:B21"/>
-    <mergeCell ref="B294:B297"/>
-    <mergeCell ref="B106:B109"/>
-    <mergeCell ref="B382:B385"/>
-    <mergeCell ref="B42:B45"/>
-    <mergeCell ref="B278:B281"/>
-    <mergeCell ref="B170:B173"/>
-    <mergeCell ref="B10:B13"/>
-    <mergeCell ref="B250:B253"/>
-    <mergeCell ref="B342:B345"/>
-    <mergeCell ref="B146:B149"/>
-    <mergeCell ref="B178:B181"/>
-    <mergeCell ref="B34:B37"/>
-    <mergeCell ref="B74:B77"/>
-    <mergeCell ref="A82:A121"/>
-    <mergeCell ref="B270:B273"/>
-    <mergeCell ref="B310:B313"/>
-    <mergeCell ref="B162:B165"/>
-    <mergeCell ref="B334:B337"/>
-    <mergeCell ref="B22:B25"/>
-    <mergeCell ref="B150:B153"/>
-    <mergeCell ref="B326:B329"/>
-    <mergeCell ref="B254:B257"/>
-    <mergeCell ref="B30:B33"/>
-    <mergeCell ref="B198:B201"/>
-    <mergeCell ref="B174:B177"/>
-    <mergeCell ref="B126:B129"/>
-    <mergeCell ref="B218:B221"/>
-    <mergeCell ref="B110:B113"/>
-    <mergeCell ref="B54:B57"/>
-    <mergeCell ref="B202:B205"/>
-    <mergeCell ref="B86:B89"/>
-    <mergeCell ref="B370:B373"/>
-    <mergeCell ref="B62:B65"/>
-    <mergeCell ref="B14:B17"/>
-    <mergeCell ref="B70:B73"/>
-    <mergeCell ref="B290:B293"/>
-    <mergeCell ref="A42:A81"/>
-    <mergeCell ref="B182:B185"/>
-    <mergeCell ref="B362:B365"/>
-    <mergeCell ref="B346:B349"/>
-    <mergeCell ref="B246:B249"/>
-    <mergeCell ref="A202:A241"/>
-    <mergeCell ref="B298:B301"/>
-    <mergeCell ref="A122:A161"/>
-    <mergeCell ref="B82:B85"/>
-    <mergeCell ref="B210:B213"/>
-    <mergeCell ref="B358:B361"/>
-    <mergeCell ref="B354:B357"/>
-    <mergeCell ref="B330:B333"/>
-    <mergeCell ref="B282:B285"/>
-    <mergeCell ref="B94:B97"/>
-    <mergeCell ref="B46:B49"/>
-    <mergeCell ref="B102:B105"/>
-    <mergeCell ref="B242:B245"/>
-    <mergeCell ref="B398:B401"/>
-    <mergeCell ref="A362:A401"/>
-    <mergeCell ref="B222:B225"/>
-    <mergeCell ref="B114:B117"/>
-    <mergeCell ref="B154:B157"/>
-    <mergeCell ref="B206:B209"/>
-    <mergeCell ref="B390:B393"/>
-    <mergeCell ref="B138:B141"/>
-    <mergeCell ref="B374:B377"/>
-    <mergeCell ref="A162:A201"/>
-    <mergeCell ref="B386:B389"/>
-    <mergeCell ref="B190:B193"/>
-    <mergeCell ref="B322:B325"/>
-    <mergeCell ref="B262:B265"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>